<commit_message>
Description : Exception handling and retry mechanism, Dynamic delay for release2 Developer Name : Snehalata Date : 08-Jul-2021
</commit_message>
<xml_diff>
--- a/Data/Output/Test_Execution_Result/07-Jul-2021/Log_Table_07-07-2021.xlsx
+++ b/Data/Output/Test_Execution_Result/07-Jul-2021/Log_Table_07-07-2021.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="1073">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="1148">
   <x:si>
     <x:t>Log_date</x:t>
   </x:si>
@@ -3274,6 +3274,231 @@
   </x:si>
   <x:si>
     <x:t>2021-07-07 12:39:03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:44:33</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:44:10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:44:11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:44:32</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:44:37</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:44:34</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:44:36</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:44:40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:44:39</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:44:43</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:44:42</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:44:48</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:44:47</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:45:16</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:44:54</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:45:15</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:45:19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:45:18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:45:24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:45:23</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:45:55</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cannot find the UI element corresponding to this selector: &lt;html app='chrome.exe' title='*' /&gt;--UiPath.UiAutomation.Activities</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:47:14</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:46:01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:47:13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>00:01:11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:47:17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:47:16</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:47:22</x:t>
+  </x:si>
+  <x:si>
+    <x:t>00:01:20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:47:21</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:47:53</x:t>
+  </x:si>
+  <x:si>
+    <x:t>00:01:51</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:48:53</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:47:59</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:48:52</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:48:55</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:49:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:48:56</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:48:59</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:49:35</x:t>
+  </x:si>
+  <x:si>
+    <x:t>00:01:36</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:50:34</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:49:40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:50:33</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:50:38</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:50:35</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:50:37</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:50:43</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:50:42</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:51:14</x:t>
+  </x:si>
+  <x:si>
+    <x:t>00:01:34</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:52:14</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:51:20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:52:13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:52:22</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:52:15</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:52:27</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:52:26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:52:38</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:52:37</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:52:45</x:t>
+  </x:si>
+  <x:si>
+    <x:t>00:01:25</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:52:44</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:52:58</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:52:57</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:53:38</x:t>
+  </x:si>
+  <x:si>
+    <x:t>00:02:17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:53:37</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:53:46</x:t>
+  </x:si>
+  <x:si>
+    <x:t>00:02:26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:53:45</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:53:51</x:t>
+  </x:si>
+  <x:si>
+    <x:t>00:02:31</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-07-07 15:53:50</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -15541,6 +15766,1758 @@
         <x:v>36</x:v>
       </x:c>
     </x:row>
+    <x:row r="207" spans="1:21">
+      <x:c r="A207" s="0" t="s">
+        <x:v>1073</x:v>
+      </x:c>
+      <x:c r="B207" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C207" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D207" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E207" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="G207" s="0" t="s">
+        <x:v>1074</x:v>
+      </x:c>
+      <x:c r="H207" s="0" t="s">
+        <x:v>1073</x:v>
+      </x:c>
+      <x:c r="I207" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="J207" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K207" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="L207" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="M207" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="N207" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="O207" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="P207" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q207" s="0" t="s">
+        <x:v>1075</x:v>
+      </x:c>
+      <x:c r="R207" s="0" t="s">
+        <x:v>1076</x:v>
+      </x:c>
+      <x:c r="S207" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T207" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="208" spans="1:21">
+      <x:c r="A208" s="0" t="s">
+        <x:v>1077</x:v>
+      </x:c>
+      <x:c r="B208" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C208" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D208" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E208" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="G208" s="0" t="s">
+        <x:v>1074</x:v>
+      </x:c>
+      <x:c r="H208" s="0" t="s">
+        <x:v>1077</x:v>
+      </x:c>
+      <x:c r="I208" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="J208" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="K208" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="M208" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N208" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O208" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P208" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q208" s="0" t="s">
+        <x:v>1078</x:v>
+      </x:c>
+      <x:c r="R208" s="0" t="s">
+        <x:v>1079</x:v>
+      </x:c>
+      <x:c r="S208" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="T208" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="209" spans="1:21">
+      <x:c r="A209" s="0" t="s">
+        <x:v>1080</x:v>
+      </x:c>
+      <x:c r="B209" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C209" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D209" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E209" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="G209" s="0" t="s">
+        <x:v>1074</x:v>
+      </x:c>
+      <x:c r="H209" s="0" t="s">
+        <x:v>1080</x:v>
+      </x:c>
+      <x:c r="I209" s="0" t="s">
+        <x:v>301</x:v>
+      </x:c>
+      <x:c r="J209" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="K209" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="M209" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="N209" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="O209" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="P209" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q209" s="0" t="s">
+        <x:v>1077</x:v>
+      </x:c>
+      <x:c r="R209" s="0" t="s">
+        <x:v>1081</x:v>
+      </x:c>
+      <x:c r="S209" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="T209" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="210" spans="1:21">
+      <x:c r="A210" s="0" t="s">
+        <x:v>1082</x:v>
+      </x:c>
+      <x:c r="B210" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C210" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D210" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E210" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="G210" s="0" t="s">
+        <x:v>1074</x:v>
+      </x:c>
+      <x:c r="H210" s="0" t="s">
+        <x:v>1082</x:v>
+      </x:c>
+      <x:c r="I210" s="0" t="s">
+        <x:v>304</x:v>
+      </x:c>
+      <x:c r="J210" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="K210" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="L210" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="M210" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="N210" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="O210" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="P210" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q210" s="0" t="s">
+        <x:v>1080</x:v>
+      </x:c>
+      <x:c r="R210" s="0" t="s">
+        <x:v>1083</x:v>
+      </x:c>
+      <x:c r="S210" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="T210" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="211" spans="1:21">
+      <x:c r="A211" s="0" t="s">
+        <x:v>1084</x:v>
+      </x:c>
+      <x:c r="B211" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C211" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D211" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E211" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F211" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="G211" s="0" t="s">
+        <x:v>1074</x:v>
+      </x:c>
+      <x:c r="H211" s="0" t="s">
+        <x:v>1084</x:v>
+      </x:c>
+      <x:c r="I211" s="0" t="s">
+        <x:v>513</x:v>
+      </x:c>
+      <x:c r="J211" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="K211" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="M211" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="N211" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="O211" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="P211" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q211" s="0" t="s">
+        <x:v>1082</x:v>
+      </x:c>
+      <x:c r="R211" s="0" t="s">
+        <x:v>1085</x:v>
+      </x:c>
+      <x:c r="S211" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="T211" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="212" spans="1:21">
+      <x:c r="A212" s="0" t="s">
+        <x:v>1086</x:v>
+      </x:c>
+      <x:c r="B212" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C212" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D212" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="E212" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="G212" s="0" t="s">
+        <x:v>1087</x:v>
+      </x:c>
+      <x:c r="H212" s="0" t="s">
+        <x:v>1086</x:v>
+      </x:c>
+      <x:c r="I212" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="J212" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K212" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="L212" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="M212" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="N212" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="O212" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="P212" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q212" s="0" t="s">
+        <x:v>1087</x:v>
+      </x:c>
+      <x:c r="R212" s="0" t="s">
+        <x:v>1088</x:v>
+      </x:c>
+      <x:c r="S212" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="T212" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="213" spans="1:21">
+      <x:c r="A213" s="0" t="s">
+        <x:v>1089</x:v>
+      </x:c>
+      <x:c r="B213" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C213" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D213" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="E213" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="G213" s="0" t="s">
+        <x:v>1087</x:v>
+      </x:c>
+      <x:c r="H213" s="0" t="s">
+        <x:v>1089</x:v>
+      </x:c>
+      <x:c r="I213" s="0" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="J213" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="K213" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="M213" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N213" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O213" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P213" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q213" s="0" t="s">
+        <x:v>1086</x:v>
+      </x:c>
+      <x:c r="R213" s="0" t="s">
+        <x:v>1090</x:v>
+      </x:c>
+      <x:c r="S213" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="T213" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="214" spans="1:21">
+      <x:c r="A214" s="0" t="s">
+        <x:v>1091</x:v>
+      </x:c>
+      <x:c r="B214" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C214" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D214" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="E214" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="G214" s="0" t="s">
+        <x:v>1087</x:v>
+      </x:c>
+      <x:c r="H214" s="0" t="s">
+        <x:v>1091</x:v>
+      </x:c>
+      <x:c r="I214" s="0" t="s">
+        <x:v>301</x:v>
+      </x:c>
+      <x:c r="J214" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="K214" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="L214" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="M214" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="N214" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="O214" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="P214" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q214" s="0" t="s">
+        <x:v>1089</x:v>
+      </x:c>
+      <x:c r="R214" s="0" t="s">
+        <x:v>1092</x:v>
+      </x:c>
+      <x:c r="S214" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="T214" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="215" spans="1:21">
+      <x:c r="A215" s="0" t="s">
+        <x:v>1093</x:v>
+      </x:c>
+      <x:c r="B215" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C215" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D215" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="E215" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="G215" s="0" t="s">
+        <x:v>1087</x:v>
+      </x:c>
+      <x:c r="H215" s="0" t="s">
+        <x:v>1093</x:v>
+      </x:c>
+      <x:c r="I215" s="0" t="s">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="J215" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="K215" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="L215" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="M215" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="N215" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="O215" s="0" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="P215" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q215" s="0" t="s">
+        <x:v>1091</x:v>
+      </x:c>
+      <x:c r="R215" s="0" t="s">
+        <x:v>727</x:v>
+      </x:c>
+      <x:c r="S215" s="0" t="s">
+        <x:v>728</x:v>
+      </x:c>
+      <x:c r="T215" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="U215" s="0" t="s">
+        <x:v>1094</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="216" spans="1:21">
+      <x:c r="A216" s="0" t="s">
+        <x:v>1095</x:v>
+      </x:c>
+      <x:c r="B216" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C216" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D216" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="E216" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="G216" s="0" t="s">
+        <x:v>1096</x:v>
+      </x:c>
+      <x:c r="H216" s="0" t="s">
+        <x:v>1095</x:v>
+      </x:c>
+      <x:c r="I216" s="0" t="s">
+        <x:v>549</x:v>
+      </x:c>
+      <x:c r="J216" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K216" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="L216" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="M216" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="N216" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="O216" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="P216" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q216" s="0" t="s">
+        <x:v>1096</x:v>
+      </x:c>
+      <x:c r="R216" s="0" t="s">
+        <x:v>1097</x:v>
+      </x:c>
+      <x:c r="S216" s="0" t="s">
+        <x:v>1098</x:v>
+      </x:c>
+      <x:c r="T216" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="217" spans="1:21">
+      <x:c r="A217" s="0" t="s">
+        <x:v>1099</x:v>
+      </x:c>
+      <x:c r="B217" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C217" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D217" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="E217" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="G217" s="0" t="s">
+        <x:v>1096</x:v>
+      </x:c>
+      <x:c r="H217" s="0" t="s">
+        <x:v>1099</x:v>
+      </x:c>
+      <x:c r="I217" s="0" t="s">
+        <x:v>556</x:v>
+      </x:c>
+      <x:c r="J217" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="K217" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="M217" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N217" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O217" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P217" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q217" s="0" t="s">
+        <x:v>1095</x:v>
+      </x:c>
+      <x:c r="R217" s="0" t="s">
+        <x:v>1100</x:v>
+      </x:c>
+      <x:c r="S217" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="T217" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="218" spans="1:21">
+      <x:c r="A218" s="0" t="s">
+        <x:v>1101</x:v>
+      </x:c>
+      <x:c r="B218" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C218" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D218" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="E218" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="G218" s="0" t="s">
+        <x:v>1096</x:v>
+      </x:c>
+      <x:c r="H218" s="0" t="s">
+        <x:v>1101</x:v>
+      </x:c>
+      <x:c r="I218" s="0" t="s">
+        <x:v>1102</x:v>
+      </x:c>
+      <x:c r="J218" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="K218" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="L218" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="M218" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="N218" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="O218" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="P218" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q218" s="0" t="s">
+        <x:v>1099</x:v>
+      </x:c>
+      <x:c r="R218" s="0" t="s">
+        <x:v>1103</x:v>
+      </x:c>
+      <x:c r="S218" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="T218" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="219" spans="1:21">
+      <x:c r="A219" s="0" t="s">
+        <x:v>1104</x:v>
+      </x:c>
+      <x:c r="B219" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C219" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D219" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="E219" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="G219" s="0" t="s">
+        <x:v>1096</x:v>
+      </x:c>
+      <x:c r="H219" s="0" t="s">
+        <x:v>1104</x:v>
+      </x:c>
+      <x:c r="I219" s="0" t="s">
+        <x:v>1105</x:v>
+      </x:c>
+      <x:c r="J219" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="K219" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="L219" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="M219" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="N219" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="O219" s="0" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="P219" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q219" s="0" t="s">
+        <x:v>1101</x:v>
+      </x:c>
+      <x:c r="R219" s="0" t="s">
+        <x:v>727</x:v>
+      </x:c>
+      <x:c r="S219" s="0" t="s">
+        <x:v>728</x:v>
+      </x:c>
+      <x:c r="T219" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="U219" s="0" t="s">
+        <x:v>1094</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="220" spans="1:21">
+      <x:c r="A220" s="0" t="s">
+        <x:v>1106</x:v>
+      </x:c>
+      <x:c r="B220" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C220" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D220" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="E220" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="G220" s="0" t="s">
+        <x:v>1107</x:v>
+      </x:c>
+      <x:c r="H220" s="0" t="s">
+        <x:v>1106</x:v>
+      </x:c>
+      <x:c r="I220" s="0" t="s">
+        <x:v>653</x:v>
+      </x:c>
+      <x:c r="J220" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K220" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="L220" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="M220" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="N220" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="O220" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="P220" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q220" s="0" t="s">
+        <x:v>1107</x:v>
+      </x:c>
+      <x:c r="R220" s="0" t="s">
+        <x:v>1108</x:v>
+      </x:c>
+      <x:c r="S220" s="0" t="s">
+        <x:v>437</x:v>
+      </x:c>
+      <x:c r="T220" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="221" spans="1:21">
+      <x:c r="A221" s="0" t="s">
+        <x:v>1109</x:v>
+      </x:c>
+      <x:c r="B221" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C221" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D221" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="E221" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="G221" s="0" t="s">
+        <x:v>1107</x:v>
+      </x:c>
+      <x:c r="H221" s="0" t="s">
+        <x:v>1109</x:v>
+      </x:c>
+      <x:c r="I221" s="0" t="s">
+        <x:v>396</x:v>
+      </x:c>
+      <x:c r="J221" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="K221" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="M221" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N221" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O221" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P221" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q221" s="0" t="s">
+        <x:v>1106</x:v>
+      </x:c>
+      <x:c r="R221" s="0" t="s">
+        <x:v>1109</x:v>
+      </x:c>
+      <x:c r="S221" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="T221" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="222" spans="1:21">
+      <x:c r="A222" s="0" t="s">
+        <x:v>1110</x:v>
+      </x:c>
+      <x:c r="B222" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C222" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D222" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="E222" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="G222" s="0" t="s">
+        <x:v>1107</x:v>
+      </x:c>
+      <x:c r="H222" s="0" t="s">
+        <x:v>1110</x:v>
+      </x:c>
+      <x:c r="I222" s="0" t="s">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="J222" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="K222" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="L222" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="M222" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="N222" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="O222" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="P222" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q222" s="0" t="s">
+        <x:v>1111</x:v>
+      </x:c>
+      <x:c r="R222" s="0" t="s">
+        <x:v>1112</x:v>
+      </x:c>
+      <x:c r="S222" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="T222" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="223" spans="1:21">
+      <x:c r="A223" s="0" t="s">
+        <x:v>1113</x:v>
+      </x:c>
+      <x:c r="B223" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C223" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D223" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="E223" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="G223" s="0" t="s">
+        <x:v>1107</x:v>
+      </x:c>
+      <x:c r="H223" s="0" t="s">
+        <x:v>1113</x:v>
+      </x:c>
+      <x:c r="I223" s="0" t="s">
+        <x:v>1114</x:v>
+      </x:c>
+      <x:c r="J223" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="K223" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="L223" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="M223" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="N223" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="O223" s="0" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="P223" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q223" s="0" t="s">
+        <x:v>1110</x:v>
+      </x:c>
+      <x:c r="R223" s="0" t="s">
+        <x:v>727</x:v>
+      </x:c>
+      <x:c r="S223" s="0" t="s">
+        <x:v>728</x:v>
+      </x:c>
+      <x:c r="T223" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="U223" s="0" t="s">
+        <x:v>729</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="224" spans="1:21">
+      <x:c r="A224" s="0" t="s">
+        <x:v>1115</x:v>
+      </x:c>
+      <x:c r="B224" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C224" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="D224" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="E224" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="G224" s="0" t="s">
+        <x:v>1116</x:v>
+      </x:c>
+      <x:c r="H224" s="0" t="s">
+        <x:v>1115</x:v>
+      </x:c>
+      <x:c r="I224" s="0" t="s">
+        <x:v>653</x:v>
+      </x:c>
+      <x:c r="J224" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K224" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="L224" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="M224" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="N224" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="O224" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="P224" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q224" s="0" t="s">
+        <x:v>1116</x:v>
+      </x:c>
+      <x:c r="R224" s="0" t="s">
+        <x:v>1117</x:v>
+      </x:c>
+      <x:c r="S224" s="0" t="s">
+        <x:v>437</x:v>
+      </x:c>
+      <x:c r="T224" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="225" spans="1:21">
+      <x:c r="A225" s="0" t="s">
+        <x:v>1118</x:v>
+      </x:c>
+      <x:c r="B225" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C225" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="D225" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="E225" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="G225" s="0" t="s">
+        <x:v>1116</x:v>
+      </x:c>
+      <x:c r="H225" s="0" t="s">
+        <x:v>1118</x:v>
+      </x:c>
+      <x:c r="I225" s="0" t="s">
+        <x:v>210</x:v>
+      </x:c>
+      <x:c r="J225" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="K225" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="M225" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N225" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O225" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P225" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q225" s="0" t="s">
+        <x:v>1119</x:v>
+      </x:c>
+      <x:c r="R225" s="0" t="s">
+        <x:v>1120</x:v>
+      </x:c>
+      <x:c r="S225" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="T225" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="226" spans="1:21">
+      <x:c r="A226" s="0" t="s">
+        <x:v>1121</x:v>
+      </x:c>
+      <x:c r="B226" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C226" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="D226" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="E226" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="G226" s="0" t="s">
+        <x:v>1116</x:v>
+      </x:c>
+      <x:c r="H226" s="0" t="s">
+        <x:v>1121</x:v>
+      </x:c>
+      <x:c r="I226" s="0" t="s">
+        <x:v>181</x:v>
+      </x:c>
+      <x:c r="J226" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="K226" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="L226" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="M226" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="N226" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="O226" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="P226" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q226" s="0" t="s">
+        <x:v>1118</x:v>
+      </x:c>
+      <x:c r="R226" s="0" t="s">
+        <x:v>1122</x:v>
+      </x:c>
+      <x:c r="S226" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="T226" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="227" spans="1:21">
+      <x:c r="A227" s="0" t="s">
+        <x:v>1123</x:v>
+      </x:c>
+      <x:c r="B227" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C227" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="D227" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="E227" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="G227" s="0" t="s">
+        <x:v>1116</x:v>
+      </x:c>
+      <x:c r="H227" s="0" t="s">
+        <x:v>1123</x:v>
+      </x:c>
+      <x:c r="I227" s="0" t="s">
+        <x:v>1124</x:v>
+      </x:c>
+      <x:c r="J227" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="K227" s="0" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="L227" s="0" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="M227" s="0" t="s">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="N227" s="0" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="O227" s="0" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="P227" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q227" s="0" t="s">
+        <x:v>1121</x:v>
+      </x:c>
+      <x:c r="R227" s="0" t="s">
+        <x:v>727</x:v>
+      </x:c>
+      <x:c r="S227" s="0" t="s">
+        <x:v>728</x:v>
+      </x:c>
+      <x:c r="T227" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="U227" s="0" t="s">
+        <x:v>729</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="228" spans="1:21">
+      <x:c r="A228" s="0" t="s">
+        <x:v>1125</x:v>
+      </x:c>
+      <x:c r="B228" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C228" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="D228" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="E228" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="G228" s="0" t="s">
+        <x:v>1126</x:v>
+      </x:c>
+      <x:c r="H228" s="0" t="s">
+        <x:v>1125</x:v>
+      </x:c>
+      <x:c r="I228" s="0" t="s">
+        <x:v>653</x:v>
+      </x:c>
+      <x:c r="J228" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="K228" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="L228" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="M228" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="N228" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="O228" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="P228" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q228" s="0" t="s">
+        <x:v>1126</x:v>
+      </x:c>
+      <x:c r="R228" s="0" t="s">
+        <x:v>1127</x:v>
+      </x:c>
+      <x:c r="S228" s="0" t="s">
+        <x:v>437</x:v>
+      </x:c>
+      <x:c r="T228" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="229" spans="1:21">
+      <x:c r="A229" s="0" t="s">
+        <x:v>1128</x:v>
+      </x:c>
+      <x:c r="B229" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C229" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="D229" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="E229" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="G229" s="0" t="s">
+        <x:v>1126</x:v>
+      </x:c>
+      <x:c r="H229" s="0" t="s">
+        <x:v>1128</x:v>
+      </x:c>
+      <x:c r="I229" s="0" t="s">
+        <x:v>181</x:v>
+      </x:c>
+      <x:c r="J229" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="K229" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="M229" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="N229" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="O229" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="P229" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q229" s="0" t="s">
+        <x:v>1129</x:v>
+      </x:c>
+      <x:c r="R229" s="0" t="s">
+        <x:v>1128</x:v>
+      </x:c>
+      <x:c r="S229" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="T229" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="230" spans="1:21">
+      <x:c r="A230" s="0" t="s">
+        <x:v>1130</x:v>
+      </x:c>
+      <x:c r="B230" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C230" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="D230" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="E230" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="G230" s="0" t="s">
+        <x:v>1126</x:v>
+      </x:c>
+      <x:c r="H230" s="0" t="s">
+        <x:v>1130</x:v>
+      </x:c>
+      <x:c r="I230" s="0" t="s">
+        <x:v>843</x:v>
+      </x:c>
+      <x:c r="J230" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="K230" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="L230" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="M230" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="N230" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="O230" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="P230" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q230" s="0" t="s">
+        <x:v>1128</x:v>
+      </x:c>
+      <x:c r="R230" s="0" t="s">
+        <x:v>1131</x:v>
+      </x:c>
+      <x:c r="S230" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="T230" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="231" spans="1:21">
+      <x:c r="A231" s="0" t="s">
+        <x:v>1132</x:v>
+      </x:c>
+      <x:c r="B231" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C231" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="D231" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="E231" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="G231" s="0" t="s">
+        <x:v>1126</x:v>
+      </x:c>
+      <x:c r="H231" s="0" t="s">
+        <x:v>1132</x:v>
+      </x:c>
+      <x:c r="I231" s="0" t="s">
+        <x:v>790</x:v>
+      </x:c>
+      <x:c r="J231" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="K231" s="0" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="L231" s="0" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="M231" s="0" t="s">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="N231" s="0" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="O231" s="0" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="P231" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q231" s="0" t="s">
+        <x:v>1130</x:v>
+      </x:c>
+      <x:c r="R231" s="0" t="s">
+        <x:v>1133</x:v>
+      </x:c>
+      <x:c r="S231" s="0" t="s">
+        <x:v>145</x:v>
+      </x:c>
+      <x:c r="T231" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="232" spans="1:21">
+      <x:c r="A232" s="0" t="s">
+        <x:v>1134</x:v>
+      </x:c>
+      <x:c r="B232" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C232" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="D232" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="E232" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="G232" s="0" t="s">
+        <x:v>1126</x:v>
+      </x:c>
+      <x:c r="H232" s="0" t="s">
+        <x:v>1134</x:v>
+      </x:c>
+      <x:c r="I232" s="0" t="s">
+        <x:v>1135</x:v>
+      </x:c>
+      <x:c r="J232" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="K232" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="L232" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="M232" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="N232" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="O232" s="0" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="P232" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q232" s="0" t="s">
+        <x:v>1132</x:v>
+      </x:c>
+      <x:c r="R232" s="0" t="s">
+        <x:v>1136</x:v>
+      </x:c>
+      <x:c r="S232" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="T232" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="233" spans="1:21">
+      <x:c r="A233" s="0" t="s">
+        <x:v>1137</x:v>
+      </x:c>
+      <x:c r="B233" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C233" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="D233" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="E233" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="G233" s="0" t="s">
+        <x:v>1126</x:v>
+      </x:c>
+      <x:c r="H233" s="0" t="s">
+        <x:v>1137</x:v>
+      </x:c>
+      <x:c r="I233" s="0" t="s">
+        <x:v>578</x:v>
+      </x:c>
+      <x:c r="J233" s="0" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="K233" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="M233" s="0" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="N233" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="O233" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="P233" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q233" s="0" t="s">
+        <x:v>1134</x:v>
+      </x:c>
+      <x:c r="R233" s="0" t="s">
+        <x:v>1138</x:v>
+      </x:c>
+      <x:c r="S233" s="0" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="T233" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="234" spans="1:21">
+      <x:c r="A234" s="0" t="s">
+        <x:v>1139</x:v>
+      </x:c>
+      <x:c r="B234" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C234" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="D234" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="E234" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="G234" s="0" t="s">
+        <x:v>1126</x:v>
+      </x:c>
+      <x:c r="H234" s="0" t="s">
+        <x:v>1139</x:v>
+      </x:c>
+      <x:c r="I234" s="0" t="s">
+        <x:v>1140</x:v>
+      </x:c>
+      <x:c r="J234" s="0" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="K234" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="M234" s="0" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="N234" s="0" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="O234" s="0" t="s">
+        <x:v>109</x:v>
+      </x:c>
+      <x:c r="P234" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q234" s="0" t="s">
+        <x:v>1137</x:v>
+      </x:c>
+      <x:c r="R234" s="0" t="s">
+        <x:v>1141</x:v>
+      </x:c>
+      <x:c r="S234" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="T234" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="235" spans="1:21">
+      <x:c r="A235" s="0" t="s">
+        <x:v>1142</x:v>
+      </x:c>
+      <x:c r="B235" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C235" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="D235" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="E235" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="G235" s="0" t="s">
+        <x:v>1126</x:v>
+      </x:c>
+      <x:c r="H235" s="0" t="s">
+        <x:v>1142</x:v>
+      </x:c>
+      <x:c r="I235" s="0" t="s">
+        <x:v>1143</x:v>
+      </x:c>
+      <x:c r="J235" s="0" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="K235" s="0" t="s">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="M235" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="N235" s="0" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="O235" s="0" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="P235" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q235" s="0" t="s">
+        <x:v>1139</x:v>
+      </x:c>
+      <x:c r="R235" s="0" t="s">
+        <x:v>1144</x:v>
+      </x:c>
+      <x:c r="S235" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="T235" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="236" spans="1:21">
+      <x:c r="A236" s="0" t="s">
+        <x:v>1145</x:v>
+      </x:c>
+      <x:c r="B236" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C236" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="D236" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="E236" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="F236" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="G236" s="0" t="s">
+        <x:v>1126</x:v>
+      </x:c>
+      <x:c r="H236" s="0" t="s">
+        <x:v>1145</x:v>
+      </x:c>
+      <x:c r="I236" s="0" t="s">
+        <x:v>1146</x:v>
+      </x:c>
+      <x:c r="J236" s="0" t="s">
+        <x:v>160</x:v>
+      </x:c>
+      <x:c r="K236" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="M236" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="N236" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="O236" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="P236" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q236" s="0" t="s">
+        <x:v>1142</x:v>
+      </x:c>
+      <x:c r="R236" s="0" t="s">
+        <x:v>1147</x:v>
+      </x:c>
+      <x:c r="S236" s="0" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="T236" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>